<commit_message>
add nodes names&cuits and invoiceId
</commit_message>
<xml_diff>
--- a/tests/Casos categorizados.xlsx
+++ b/tests/Casos categorizados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\agents\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\agents\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADE116E-7746-4B9A-AECE-F758030077A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EBDAAC-2486-4DF0-9DDE-0C2918129915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8261,19 +8261,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C147" sqref="C147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="62.42578125" customWidth="1"/>
     <col min="2" max="2" width="68.28515625" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="50.85546875" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="36.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="50.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>